<commit_message>
Primo tentativo di almeno FAR FINTA di risolvere il problema della fascia iniziale
</commit_message>
<xml_diff>
--- a/PS-VRP/Archivio/Archivio output/errori_compatibilità.xlsx
+++ b/PS-VRP/Archivio/Archivio output/errori_compatibilità.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>252466</v>
+        <v>252417</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -457,29 +457,9 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>252418</v>
+        <v>252980</v>
       </c>
       <c r="B3" t="inlineStr">
-        <is>
-          <t>nessuna compatibilità con alcuna macchina</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>252417</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>nessuna compatibilità con alcuna macchina</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>252980</v>
-      </c>
-      <c r="B5" t="inlineStr">
         <is>
           <t>nessuna compatibilità con alcuna macchina</t>
         </is>

</xml_diff>